<commit_message>
corrections according to list RH
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_orgNames_2023.xlsx
+++ b/data/xlsx/Baernreither_orgNames_2023.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofaichner/Documents/GitHub/baernreither-data/data/xlsx/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0A3424-3CF5-E442-9B67-83C26A1E3B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Tabelle1" sheetId="1" r:id="rId4"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="cr9iom4sTbZZpAtw5R4I3V7HGloPmJ38awLU2ZnUpI8="/>
@@ -16,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="535">
   <si>
     <t>Spalte 1</t>
   </si>
@@ -73,18 +82,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="Dreibund" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/4150632-7</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -96,18 +112,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="Freimaurer" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/4123227-6</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -188,18 +211,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="HotelSacher" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/3046318-X</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -247,18 +277,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="KaschauOderbergerBahn" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/1087469716</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -273,18 +310,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="SanPaolo" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/4637768-2</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -378,26 +422,26 @@
   <si>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
       </rPr>
       <t>&lt;orgName key="LandtagNiederoesterreich" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://d-nb.info/gnd/1223443-6</t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
       </rPr>
       <t>"&gt;</t>
     </r>
@@ -423,26 +467,26 @@
   <si>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
       </rPr>
       <t>&lt;orgName key="Landwehr" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://d-nb.info/gnd/5057819-4</t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
       </rPr>
       <t>"&gt;</t>
     </r>
@@ -623,18 +667,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="Ministerrat" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/4236755-4</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -695,26 +746,26 @@
   <si>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
       </rPr>
       <t>&lt;orgName key="OberlandesgerichtPrag" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://d-nb.info/gnd/7553054-5</t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
       </rPr>
       <t>"&gt;</t>
     </r>
@@ -751,18 +802,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="Patentamt" ref= "</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/41792-0</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -795,18 +853,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="AllgemeineZeitung" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/1368786642</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -817,9 +882,6 @@
     <t>AltoAdige</t>
   </si>
   <si>
-    <t>&lt;orgName key="AltoAdige" ref=""&gt;</t>
-  </si>
-  <si>
     <t>Presse/Arbeiterzeitung</t>
   </si>
   <si>
@@ -881,18 +943,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="Fremdenblatt" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/1086227905</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -1044,9 +1113,6 @@
     <t>Popolo</t>
   </si>
   <si>
-    <t>&lt;orgName key="Popolo" ref=""&gt;</t>
-  </si>
-  <si>
     <t>Presse/Prager Tagblatt</t>
   </si>
   <si>
@@ -1150,18 +1216,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="EisernerRing" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/5248775-1</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -1218,18 +1291,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="DeutscherKlub" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/1289674884</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -1387,9 +1467,6 @@
     <t>Reichsrat/Abgeordnetenhaus/Parteien/Rumänenklub</t>
   </si>
   <si>
-    <t>Rumänenklub</t>
-  </si>
-  <si>
     <t>&lt;orgName key="Rumaenenklub"&gt;</t>
   </si>
   <si>
@@ -1520,18 +1597,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="Justizausschuss" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/5080590-3</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -1539,9 +1623,6 @@
     <t>Reichsrat/Abgeordnetenhaus/Notstandsausschuss</t>
   </si>
   <si>
-    <t>Nostandsausschuss</t>
-  </si>
-  <si>
     <t>&lt;orgName key="Notstandsausschuss" ref=""&gt;</t>
   </si>
   <si>
@@ -1636,18 +1717,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="Staatsschuldenkontrollkommission" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/5054264-3</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -1833,18 +1921,25 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t>&lt;orgName key="WienerMusikverein" ref="</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://d-nb.info/gnd/4580165-4</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"&gt;</t>
     </r>
   </si>
@@ -1880,258 +1975,352 @@
   </si>
   <si>
     <t>&lt;orgName key="VereinfuerSocialpolitik" ref="https://d-nb.info/gnd/1012156-0"&gt;</t>
+  </si>
+  <si>
+    <t>Notstandsausschuss</t>
+  </si>
+  <si>
+    <t>Rumaenenklub</t>
+  </si>
+  <si>
+    <t>https://d-nb.info/gnd/4142078-0 </t>
+  </si>
+  <si>
+    <t>&lt;orgName key="AltoAdige" ref="https://d-nb.info/gnd/4142078-0"&gt;</t>
+  </si>
+  <si>
+    <t>https://d-nb.info/gnd/4777777-1 </t>
+  </si>
+  <si>
+    <t>&lt;orgName key="Popolo" ref="https://d-nb.info/gnd/4777777-1"&gt;</t>
+  </si>
+  <si>
+    <t>https://d-nb.info/gnd/4271516-7 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="44">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="48">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Lato"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF4160A5"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Lato"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF4160A5"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Lato"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF0563C1"/>
       <name val="Lato"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Lato"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Lato"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF0563C1"/>
       <name val="Lato"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF1155CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri, sans-serif"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF1155CC"/>
+      <name val="Calibri, sans-serif"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2139,7 +2328,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2161,332 +2350,233 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF5B9BD5"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF5B9BD5"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF5B9BD5"/>
       </right>
       <top style="thin">
         <color rgb="FF5B9BD5"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="71">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="34" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="34" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="38" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="39" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="40" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="41" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="42" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="43" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBDD6EE"/>
+          <bgColor rgb="FFBDD6EE"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDEEAF6"/>
+          <bgColor rgb="FFDEEAF6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4"/>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDEEAF6"/>
-          <bgColor rgb="FFDEEAF6"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBDD6EE"/>
-          <bgColor rgb="FFBDD6EE"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Tabelle1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Tabelle1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D148" displayName="Table_1" name="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:D148">
   <tableColumns count="4">
-    <tableColumn name="Spalte 1" id="1"/>
-    <tableColumn name="Spalte 2" id="2"/>
-    <tableColumn name="key=wert" id="3"/>
-    <tableColumn name="Spalte4" id="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Spalte 1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Spalte 2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="key=wert"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Spalte4"/>
   </tableColumns>
-  <tableStyleInfo name="Tabelle1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Tabelle1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -2676,27 +2766,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1081"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="165" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="73.14"/>
-    <col customWidth="1" min="2" max="2" width="31.71"/>
-    <col customWidth="1" min="3" max="3" width="26.14"/>
-    <col customWidth="1" min="4" max="4" width="94.71"/>
-    <col customWidth="1" min="5" max="26" width="10.71"/>
+    <col min="1" max="1" width="73.1640625" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="45.1640625" customWidth="1"/>
+    <col min="4" max="4" width="94.6640625" customWidth="1"/>
+    <col min="5" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2710,7 +2802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="16">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2724,7 +2816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="32">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -2738,7 +2830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="16">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -2752,7 +2844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="16">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -2766,7 +2858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" ht="16">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
@@ -2780,7 +2872,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" ht="16">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -2794,7 +2886,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" ht="16">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -2808,7 +2900,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" ht="16">
       <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
@@ -2822,7 +2914,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" ht="16">
       <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
@@ -2834,7 +2926,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" ht="16">
       <c r="A11" s="5" t="s">
         <v>37</v>
       </c>
@@ -2848,7 +2940,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" ht="16">
       <c r="A12" s="5" t="s">
         <v>40</v>
       </c>
@@ -2858,15 +2950,15 @@
       <c r="C12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" ht="16">
       <c r="A13" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -2876,7 +2968,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" ht="16">
       <c r="A14" s="3" t="s">
         <v>48</v>
       </c>
@@ -2890,21 +2982,21 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:4" ht="16">
+      <c r="A15" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" ht="16">
       <c r="A16" s="5" t="s">
         <v>56</v>
       </c>
@@ -2918,25 +3010,25 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" ht="16">
       <c r="A17" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>60</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" ht="16">
       <c r="A18" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>64</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -2946,7 +3038,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" ht="32">
       <c r="A19" s="3" t="s">
         <v>67</v>
       </c>
@@ -2960,25 +3052,25 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="19" t="s">
+    <row r="20" spans="1:4">
+      <c r="A20" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" ht="16">
       <c r="A21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>76</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -2988,7 +3080,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" ht="16">
       <c r="A22" s="3" t="s">
         <v>79</v>
       </c>
@@ -3002,11 +3094,11 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" ht="16">
       <c r="A23" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="22"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="3" t="s">
         <v>84</v>
       </c>
@@ -3014,7 +3106,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" ht="16">
       <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
@@ -3026,147 +3118,147 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="13" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="13" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:4">
+      <c r="A27" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="26" t="s">
+    <row r="28" spans="1:4">
+      <c r="A28" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="27" t="s">
+    <row r="29" spans="1:4">
+      <c r="A29" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="28" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="27" t="s">
+    <row r="30" spans="1:4">
+      <c r="A30" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="28" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="27" t="s">
+    <row r="31" spans="1:4">
+      <c r="A31" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="28" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="27" t="s">
+    <row r="32" spans="1:4">
+      <c r="A32" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="70" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="28" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="27" t="s">
+    <row r="33" spans="1:26">
+      <c r="A33" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="28" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="27" t="s">
+    <row r="34" spans="1:26">
+      <c r="A34" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="28" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:26" ht="16">
       <c r="A35" s="5" t="s">
         <v>128</v>
       </c>
@@ -3180,11 +3272,11 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:26" ht="16">
       <c r="A36" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="20" t="s">
         <v>133</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -3194,7 +3286,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:26" ht="16">
       <c r="A37" s="3" t="s">
         <v>136</v>
       </c>
@@ -3208,117 +3300,117 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:26" ht="16">
       <c r="A38" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C38" s="32" t="s">
+      <c r="C38" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="34" t="s">
+    <row r="39" spans="1:26" ht="16">
+      <c r="A39" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="37"/>
-      <c r="N39" s="37"/>
-      <c r="O39" s="37"/>
-      <c r="P39" s="37"/>
-      <c r="Q39" s="37"/>
-      <c r="R39" s="37"/>
-      <c r="S39" s="37"/>
-      <c r="T39" s="37"/>
-      <c r="U39" s="37"/>
-      <c r="V39" s="37"/>
-      <c r="W39" s="37"/>
-      <c r="X39" s="37"/>
-      <c r="Y39" s="37"/>
-      <c r="Z39" s="37"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="38" t="s">
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="33"/>
+      <c r="R39" s="33"/>
+      <c r="S39" s="33"/>
+      <c r="T39" s="33"/>
+      <c r="U39" s="33"/>
+      <c r="V39" s="33"/>
+      <c r="W39" s="33"/>
+      <c r="X39" s="33"/>
+      <c r="Y39" s="33"/>
+      <c r="Z39" s="33"/>
+    </row>
+    <row r="40" spans="1:26" ht="16">
+      <c r="A40" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="38" t="s">
+    <row r="41" spans="1:26" ht="32">
+      <c r="A41" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="12" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="38" t="s">
+    <row r="42" spans="1:26" ht="32">
+      <c r="A42" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="12" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:26" ht="16">
       <c r="A43" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="68" t="s">
         <v>161</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="16" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:26" ht="16">
       <c r="A44" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="34" t="s">
         <v>164</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -3328,7 +3420,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:26" ht="16">
       <c r="A45" s="3" t="s">
         <v>167</v>
       </c>
@@ -3340,25 +3432,25 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:26" ht="16">
       <c r="A46" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="17" t="s">
         <v>171</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="D46" s="40" t="s">
+      <c r="D46" s="35" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:26" ht="16">
       <c r="A47" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="20" t="s">
         <v>175</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -3368,35 +3460,35 @@
         <v>177</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="41" t="s">
+    <row r="48" spans="1:26" ht="16">
+      <c r="A48" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="B48" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="C48" s="43" t="s">
+      <c r="C48" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="D48" s="44" t="s">
+      <c r="D48" s="39" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="45" t="s">
+    <row r="49" spans="1:26" ht="16">
+      <c r="A49" s="40" t="s">
         <v>182</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="12" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:26" ht="16">
       <c r="A50" s="3" t="s">
         <v>186</v>
       </c>
@@ -3406,29 +3498,29 @@
       <c r="C50" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="D50" s="21" t="s">
+      <c r="D50" s="20" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:26" ht="16">
       <c r="A51" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B51" s="46" t="s">
+      <c r="B51" s="41" t="s">
         <v>191</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="D51" s="16" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:26" ht="16">
       <c r="A52" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B52" s="46" t="s">
+      <c r="B52" s="41" t="s">
         <v>194</v>
       </c>
       <c r="C52" s="5" t="s">
@@ -3438,11 +3530,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:26" ht="16">
       <c r="A53" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B53" s="47"/>
+      <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
         <v>197</v>
       </c>
@@ -3450,431 +3542,435 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:26" ht="32">
       <c r="A54" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B54" s="48" t="s">
+      <c r="B54" s="42" t="s">
         <v>200</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="16" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:26" ht="16">
       <c r="A55" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B55" s="3"/>
+      <c r="B55" s="67" t="s">
+        <v>530</v>
+      </c>
       <c r="C55" s="3" t="s">
         <v>204</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" ht="16">
+      <c r="A56" s="3" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="3" t="s">
+      <c r="B56" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="C56" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="D56" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D56" s="2" t="s">
+    </row>
+    <row r="57" spans="1:26" ht="16">
+      <c r="A57" s="3" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="C57" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="D57" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D57" s="2" t="s">
+    </row>
+    <row r="58" spans="1:26" ht="16">
+      <c r="A58" s="5" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="5" t="s">
+      <c r="B58" s="5"/>
+      <c r="C58" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B58" s="47"/>
-      <c r="C58" s="5" t="s">
+      <c r="D58" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="D58" s="7" t="s">
+    </row>
+    <row r="59" spans="1:26" ht="16">
+      <c r="A59" s="3" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D59" s="2" t="s">
+    </row>
+    <row r="60" spans="1:26" ht="16">
+      <c r="A60" s="5" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="5" t="s">
+      <c r="B60" s="43"/>
+      <c r="C60" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="B60" s="49"/>
-      <c r="C60" s="5" t="s">
+      <c r="D60" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="D60" s="11" t="s">
+    </row>
+    <row r="61" spans="1:26" ht="16">
+      <c r="A61" s="8" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="8" t="s">
+      <c r="B61" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="B61" s="50" t="s">
+      <c r="C61" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="D61" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="D61" s="10" t="s">
+    </row>
+    <row r="62" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A62" s="45" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="51" t="s">
+      <c r="B62" s="46" t="s">
         <v>227</v>
       </c>
-      <c r="B62" s="52" t="s">
+      <c r="C62" s="45" t="s">
         <v>228</v>
       </c>
-      <c r="C62" s="51" t="s">
+      <c r="D62" s="47" t="s">
         <v>229</v>
       </c>
-      <c r="D62" s="53" t="s">
+      <c r="E62" s="33"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="33"/>
+      <c r="I62" s="33"/>
+      <c r="J62" s="33"/>
+      <c r="K62" s="33"/>
+      <c r="L62" s="33"/>
+      <c r="M62" s="33"/>
+      <c r="N62" s="33"/>
+      <c r="O62" s="33"/>
+      <c r="P62" s="33"/>
+      <c r="Q62" s="33"/>
+      <c r="R62" s="33"/>
+      <c r="S62" s="33"/>
+      <c r="T62" s="33"/>
+      <c r="U62" s="33"/>
+      <c r="V62" s="33"/>
+      <c r="W62" s="33"/>
+      <c r="X62" s="33"/>
+      <c r="Y62" s="33"/>
+      <c r="Z62" s="33"/>
+    </row>
+    <row r="63" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A63" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="37"/>
-      <c r="I62" s="37"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="37"/>
-      <c r="L62" s="37"/>
-      <c r="M62" s="37"/>
-      <c r="N62" s="37"/>
-      <c r="O62" s="37"/>
-      <c r="P62" s="37"/>
-      <c r="Q62" s="37"/>
-      <c r="R62" s="37"/>
-      <c r="S62" s="37"/>
-      <c r="T62" s="37"/>
-      <c r="U62" s="37"/>
-      <c r="V62" s="37"/>
-      <c r="W62" s="37"/>
-      <c r="X62" s="37"/>
-      <c r="Y62" s="37"/>
-      <c r="Z62" s="37"/>
-    </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="26" t="s">
+      <c r="B63" s="24"/>
+      <c r="C63" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="B63" s="54"/>
-      <c r="C63" s="26" t="s">
+      <c r="D63" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="D63" s="7" t="s">
+    </row>
+    <row r="64" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A64" s="24" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="26" t="s">
+      <c r="B64" s="48" t="s">
         <v>234</v>
       </c>
-      <c r="B64" s="55" t="s">
+      <c r="C64" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="C64" s="26" t="s">
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A65" s="24" t="s">
         <v>236</v>
       </c>
-      <c r="D64" s="7"/>
-    </row>
-    <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="26" t="s">
+      <c r="B65" s="48" t="s">
         <v>237</v>
       </c>
-      <c r="B65" s="55" t="s">
+      <c r="C65" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="C65" s="26" t="s">
+      <c r="D65" s="7"/>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A66" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="D65" s="7"/>
-    </row>
-    <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="27" t="s">
+      <c r="B66" s="27"/>
+      <c r="C66" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="B66" s="56"/>
-      <c r="C66" s="29" t="s">
+      <c r="D66" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="D66" s="7" t="s">
+    </row>
+    <row r="67" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A67" s="3" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="D67" s="2" t="s">
+    </row>
+    <row r="68" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A68" s="3" t="s">
         <v>245</v>
-      </c>
-    </row>
-    <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D68" s="2" t="s">
+    </row>
+    <row r="69" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A69" s="25" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="27" t="s">
+      <c r="B69" s="49"/>
+      <c r="C69" s="27" t="s">
         <v>249</v>
       </c>
-      <c r="B69" s="57"/>
-      <c r="C69" s="29" t="s">
+      <c r="D69" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="D69" s="30" t="s">
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A70" s="8" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="8" t="s">
+      <c r="B70" s="50"/>
+      <c r="C70" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="B70" s="58"/>
-      <c r="C70" s="8" t="s">
+      <c r="D70" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="D70" s="40" t="s">
+    </row>
+    <row r="71" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A71" s="3" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="3" t="s">
+      <c r="B71" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="C71" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="D71" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D71" s="2" t="s">
+    </row>
+    <row r="72" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A72" s="3" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="3" t="s">
+      <c r="B72" s="67" t="s">
         <v>259</v>
       </c>
-      <c r="B72" s="21" t="s">
+      <c r="C72" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="D72" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D72" s="2" t="s">
+    </row>
+    <row r="73" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A73" s="3" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="3" t="s">
+      <c r="B73" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="C73" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="D73" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D73" s="2" t="s">
+    </row>
+    <row r="74" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A74" s="3" t="s">
         <v>266</v>
-      </c>
-    </row>
-    <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="3" t="s">
-        <v>267</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D74" s="2" t="s">
+    </row>
+    <row r="75" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A75" s="3" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="3" t="s">
+      <c r="B75" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="C75" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="D75" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D75" s="2" t="s">
+    </row>
+    <row r="76" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A76" s="3" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="3" t="s">
+      <c r="B76" s="67" t="s">
+        <v>532</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3" t="s">
+      <c r="D76" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A77" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="B77" s="4" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="D77" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C77" s="3" t="s">
+    </row>
+    <row r="78" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A78" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="B78" s="50"/>
+      <c r="C78" s="8" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="8" t="s">
+      <c r="D78" s="35" t="s">
         <v>281</v>
       </c>
-      <c r="B78" s="58"/>
-      <c r="C78" s="8" t="s">
+    </row>
+    <row r="79" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A79" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="D78" s="40" t="s">
+      <c r="B79" s="50"/>
+      <c r="C79" s="8" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="8" t="s">
+      <c r="D79" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="B79" s="58"/>
-      <c r="C79" s="8" t="s">
+    </row>
+    <row r="80" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A80" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="D79" s="40" t="s">
+      <c r="B80" s="6" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="D80" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="C80" s="5" t="s">
+    </row>
+    <row r="81" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A81" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="5" t="s">
-        <v>291</v>
       </c>
       <c r="B81" s="6"/>
       <c r="C81" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A82" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="B82" s="20" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="3" t="s">
+      <c r="C82" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B82" s="21" t="s">
+      <c r="D82" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C82" s="3" t="s">
+    </row>
+    <row r="83" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A83" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="B83" s="4" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="D83" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C83" s="3" t="s">
+    </row>
+    <row r="84" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A84" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="B84" s="51"/>
+      <c r="C84" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="D84" s="7" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="B84" s="59"/>
-      <c r="C84" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" spans="1:4" ht="15.75" customHeight="1">
       <c r="A85" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B85" s="21" t="s">
+      <c r="B85" s="20" t="s">
         <v>187</v>
       </c>
       <c r="C85" s="3" t="s">
@@ -3884,877 +3980,879 @@
         <v>189</v>
       </c>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" spans="1:4" ht="15.75" customHeight="1">
       <c r="A86" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B86" s="69" t="s">
+        <v>303</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="B86" s="21" t="s">
+      <c r="D86" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C86" s="3" t="s">
+    </row>
+    <row r="87" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A87" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="B87" s="52" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="8" t="s">
+      <c r="C87" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="B87" s="60" t="s">
+      <c r="D87" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="C87" s="8" t="s">
+    </row>
+    <row r="88" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A88" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="D87" s="10" t="s">
+      <c r="B88" s="20" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="B88" s="21" t="s">
+      <c r="D88" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C88" s="3" t="s">
+    </row>
+    <row r="89" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A89" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="32" t="s">
+      <c r="D89" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B89" s="2"/>
-      <c r="C89" s="61" t="s">
+    </row>
+    <row r="90" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A90" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="D89" s="33" t="s">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="3" t="s">
+      <c r="D90" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B90" s="2"/>
-      <c r="C90" s="61" t="s">
+    </row>
+    <row r="91" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A91" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="B91" s="4" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="3" t="s">
+      <c r="C91" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="D91" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C91" s="3" t="s">
+    </row>
+    <row r="92" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A92" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="B92" s="6" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="5" t="s">
+      <c r="C92" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="D92" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="C92" s="5" t="s">
+    </row>
+    <row r="93" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A93" s="5" t="s">
         <v>328</v>
-      </c>
-      <c r="D92" s="17" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="5" t="s">
-        <v>330</v>
       </c>
       <c r="B93" s="6"/>
       <c r="C93" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A94" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="D93" s="11" t="s">
+      <c r="B94" s="20" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="3" t="s">
+      <c r="C94" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="B94" s="21" t="s">
+      <c r="D94" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="C94" s="3" t="s">
+    </row>
+    <row r="95" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A95" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="B95" s="4" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="D95" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="C95" s="3" t="s">
+    </row>
+    <row r="96" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A96" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="B96" s="20" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="B96" s="21" t="s">
+      <c r="D96" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C96" s="3" t="s">
+    </row>
+    <row r="97" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A97" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="B97" s="7"/>
+      <c r="C97" s="5" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="5" t="s">
+      <c r="D97" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="B97" s="62"/>
-      <c r="C97" s="5" t="s">
+    </row>
+    <row r="98" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A98" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="D97" s="7" t="s">
+      <c r="B98" s="7"/>
+      <c r="C98" s="5" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="5" t="s">
+      <c r="D98" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="B98" s="62"/>
-      <c r="C98" s="5" t="s">
+    </row>
+    <row r="99" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A99" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="D98" s="7" t="s">
+      <c r="B99" s="7"/>
+      <c r="C99" s="5" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="5" t="s">
+      <c r="D99" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="B99" s="62"/>
-      <c r="C99" s="5" t="s">
+    </row>
+    <row r="100" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A100" s="3" t="s">
         <v>352</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="3" t="s">
-        <v>354</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A101" s="25" t="s">
         <v>355</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="B101" s="53"/>
+      <c r="C101" s="27" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="27" t="s">
+      <c r="D101" s="28" t="s">
         <v>357</v>
       </c>
-      <c r="B101" s="63"/>
-      <c r="C101" s="29" t="s">
+    </row>
+    <row r="102" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A102" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="D101" s="30" t="s">
+      <c r="B102" s="7"/>
+      <c r="C102" s="5" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="5" t="s">
+      <c r="D102" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="B102" s="62"/>
-      <c r="C102" s="5" t="s">
+    </row>
+    <row r="103" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A103" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="D102" s="7" t="s">
+      <c r="B103" s="7"/>
+      <c r="C103" s="5" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="5" t="s">
+      <c r="D103" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="B103" s="62"/>
-      <c r="C103" s="5" t="s">
+    </row>
+    <row r="104" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A104" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="D103" s="7" t="s">
+      <c r="B104" s="2"/>
+      <c r="C104" s="3" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="3" t="s">
+      <c r="D104" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B104" s="2"/>
-      <c r="C104" s="32" t="s">
+    </row>
+    <row r="105" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A105" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="D104" s="33" t="s">
+      <c r="B105" s="20" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="B105" s="21" t="s">
+      <c r="D105" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="C105" s="3" t="s">
+    </row>
+    <row r="106" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A106" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="B106" s="11"/>
+      <c r="C106" s="8" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="8" t="s">
+      <c r="D106" s="35" t="s">
         <v>373</v>
       </c>
-      <c r="B106" s="12"/>
-      <c r="C106" s="8" t="s">
+    </row>
+    <row r="107" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A107" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="D106" s="40" t="s">
+      <c r="B107" s="20" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="B107" s="21" t="s">
+      <c r="D107" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C107" s="3" t="s">
+    </row>
+    <row r="108" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A108" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="B108" s="11"/>
+      <c r="C108" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="D108" s="35" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="8" t="s">
+    <row r="109" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A109" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="B108" s="12"/>
-      <c r="C108" s="8" t="s">
+      <c r="B109" s="11"/>
+      <c r="C109" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="D108" s="40" t="s">
+      <c r="D109" s="35" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="8" t="s">
+    <row r="110" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A110" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="B109" s="12"/>
-      <c r="C109" s="8" t="s">
+      <c r="B110" s="20" t="s">
         <v>384</v>
       </c>
-      <c r="D109" s="40" t="s">
+      <c r="C110" s="3" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="3" t="s">
+      <c r="D110" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B110" s="21" t="s">
+    </row>
+    <row r="111" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A111" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="B111" s="20"/>
+      <c r="C111" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="D110" s="2" t="s">
+      <c r="D111" s="2" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="32" t="s">
+    <row r="112" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A112" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="B111" s="21"/>
-      <c r="C111" s="32" t="s">
+      <c r="B112" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="D111" s="33" t="s">
+      <c r="C112" s="3" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="3" t="s">
+      <c r="D112" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B112" s="21" t="s">
+    </row>
+    <row r="113" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A113" s="5" t="s">
         <v>394</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="5" t="s">
-        <v>397</v>
       </c>
       <c r="B113" s="6"/>
       <c r="C113" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A114" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B114" s="20" t="s">
         <v>398</v>
       </c>
-      <c r="D113" s="7" t="s">
+      <c r="C114" s="3" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="3" t="s">
+      <c r="D114" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B114" s="21" t="s">
+    </row>
+    <row r="115" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A115" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="B115" s="20" t="s">
         <v>402</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="C115" s="3" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="3" t="s">
+      <c r="D115" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B115" s="21" t="s">
+    </row>
+    <row r="116" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A116" s="3" t="s">
         <v>405</v>
-      </c>
-      <c r="C115" s="32" t="s">
-        <v>406</v>
-      </c>
-      <c r="D115" s="33" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="3" t="s">
-        <v>408</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A117" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B117" s="20" t="s">
         <v>409</v>
       </c>
-      <c r="D116" s="2" t="s">
+      <c r="C117" s="3" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="3" t="s">
+      <c r="D117" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="B117" s="21" t="s">
+    </row>
+    <row r="118" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A118" s="40" t="s">
         <v>412</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="B118" s="54" t="s">
         <v>413</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="C118" s="12" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="45" t="s">
+      <c r="D118" s="12" t="s">
         <v>415</v>
       </c>
-      <c r="B118" s="64" t="s">
+    </row>
+    <row r="119" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A119" s="25" t="s">
         <v>416</v>
       </c>
-      <c r="C118" s="13" t="s">
+      <c r="B119" s="49"/>
+      <c r="C119" s="27" t="s">
         <v>417</v>
       </c>
-      <c r="D118" s="13" t="s">
+      <c r="D119" s="28" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="27" t="s">
+    <row r="120" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A120" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="B119" s="57"/>
-      <c r="C119" s="29" t="s">
+      <c r="B120" s="52" t="s">
         <v>420</v>
       </c>
-      <c r="D119" s="30" t="s">
+      <c r="C120" s="8" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="8" t="s">
+      <c r="D120" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="B120" s="60" t="s">
+    </row>
+    <row r="121" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A121" s="3" t="s">
         <v>423</v>
-      </c>
-      <c r="C120" s="8" t="s">
-        <v>424</v>
-      </c>
-      <c r="D120" s="10" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="3" t="s">
-        <v>426</v>
       </c>
       <c r="B121" s="4"/>
       <c r="C121" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A122" s="55" t="s">
+        <v>425</v>
+      </c>
+      <c r="B122" s="56" t="s">
+        <v>426</v>
+      </c>
+      <c r="C122" s="57" t="s">
         <v>427</v>
       </c>
-      <c r="D121" s="2" t="s">
+      <c r="D122" s="58" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="65" t="s">
+    <row r="123" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A123" s="55" t="s">
         <v>429</v>
       </c>
-      <c r="B122" s="66" t="s">
+      <c r="B123" s="59"/>
+      <c r="C123" s="57" t="s">
         <v>430</v>
       </c>
-      <c r="C122" s="67" t="s">
+      <c r="D123" s="58" t="s">
         <v>431</v>
       </c>
-      <c r="D122" s="68" t="s">
+    </row>
+    <row r="124" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A124" s="60" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="65" t="s">
+      <c r="B124" s="61"/>
+      <c r="C124" s="60" t="s">
         <v>433</v>
       </c>
-      <c r="B123" s="69"/>
-      <c r="C123" s="67" t="s">
+      <c r="D124" s="18" t="s">
         <v>434</v>
       </c>
-      <c r="D123" s="68" t="s">
+    </row>
+    <row r="125" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A125" s="3" t="s">
         <v>435</v>
-      </c>
-    </row>
-    <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="70" t="s">
-        <v>436</v>
-      </c>
-      <c r="B124" s="71"/>
-      <c r="C124" s="70" t="s">
-        <v>437</v>
-      </c>
-      <c r="D124" s="19" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="3" t="s">
-        <v>439</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" s="3" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="126" ht="15.75" customHeight="1">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="15.75" customHeight="1">
       <c r="A126" s="3" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A127" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C127" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="D126" s="2" t="s">
+      <c r="D127" s="2" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="3" t="s">
+    <row r="128" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A128" s="62" t="s">
         <v>445</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="63" t="s">
         <v>446</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="C128" s="62" t="s">
         <v>447</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="D128" s="2" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="72" t="s">
+    <row r="129" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A129" s="3" t="s">
         <v>449</v>
-      </c>
-      <c r="B128" s="73" t="s">
-        <v>450</v>
-      </c>
-      <c r="C128" s="72" t="s">
-        <v>451</v>
-      </c>
-      <c r="D128" s="61" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="3" t="s">
-        <v>453</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A130" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="C130" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="D129" s="2" t="s">
+      <c r="D130" s="16" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="5" t="s">
+    <row r="131" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A131" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="B130" s="6" t="s">
+      <c r="B131" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="C130" s="5" t="s">
+      <c r="C131" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="D130" s="17" t="s">
+      <c r="D131" s="7" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="5" t="s">
+    <row r="132" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A132" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="B131" s="6" t="s">
+      <c r="B132" s="20" t="s">
         <v>461</v>
       </c>
-      <c r="C131" s="5" t="s">
+      <c r="C132" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="D131" s="11" t="s">
+      <c r="D132" s="2" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="3" t="s">
+    <row r="133" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A133" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="B132" s="21" t="s">
+      <c r="B133" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="C132" s="32" t="s">
+      <c r="C133" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="D132" s="2" t="s">
+      <c r="D133" s="2" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="3" t="s">
+    <row r="134" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A134" s="3" t="s">
         <v>468</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="C133" s="3" t="s">
+      <c r="C134" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="D133" s="2" t="s">
+      <c r="D134" s="2" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="3" t="s">
+    <row r="135" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A135" s="3" t="s">
         <v>472</v>
-      </c>
-      <c r="B134" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="3" t="s">
-        <v>476</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" s="3" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="136" ht="15.75" customHeight="1">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="15.75" customHeight="1">
       <c r="A136" s="3" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A137" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="B137" s="67" t="s">
+        <v>534</v>
+      </c>
+      <c r="C137" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="D137" s="35" t="s">
         <v>480</v>
       </c>
-      <c r="D136" s="2" t="s">
+    </row>
+    <row r="138" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A138" s="5" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="8" t="s">
+      <c r="B138" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="B137" s="74"/>
-      <c r="C137" s="8" t="s">
+      <c r="C138" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="D137" s="40" t="s">
+      <c r="D138" s="7" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="5" t="s">
+    <row r="139" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A139" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="B138" s="6" t="s">
+      <c r="B139" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="C139" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="D138" s="7" t="s">
+      <c r="D139" s="2" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="3" t="s">
+    <row r="140" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A140" s="12" t="s">
         <v>489</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B140" s="13" t="s">
         <v>490</v>
       </c>
-      <c r="C139" s="3" t="s">
+      <c r="C140" s="12" t="s">
         <v>491</v>
       </c>
-      <c r="D139" s="2" t="s">
+      <c r="D140" s="12" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="13" t="s">
+    <row r="141" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A141" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="B140" s="14" t="s">
+      <c r="B141" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="C140" s="13" t="s">
+      <c r="C141" s="3" t="s">
         <v>495</v>
       </c>
-      <c r="D140" s="13" t="s">
+      <c r="D141" s="2" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="3" t="s">
+    <row r="142" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A142" s="3" t="s">
         <v>497</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>498</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="3" t="s">
-        <v>501</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A143" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="D143" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="D142" s="2" t="s">
+    </row>
+    <row r="144" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A144" s="3" t="s">
         <v>502</v>
-      </c>
-    </row>
-    <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="B143" s="4" t="s">
-        <v>504</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="3" t="s">
-        <v>506</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A145" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="B145" s="51"/>
+      <c r="C145" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="D145" s="7" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A146" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="D144" s="2" t="s">
+      <c r="B146" s="4" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="5" t="s">
+      <c r="C146" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="B145" s="59"/>
-      <c r="C145" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="D145" s="7" t="s">
+      <c r="D146" s="2" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="3" t="s">
+    <row r="147" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A147" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="51"/>
+      <c r="C147" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="C146" s="3" t="s">
+      <c r="D147" s="7" t="s">
         <v>512</v>
       </c>
-      <c r="D146" s="2" t="s">
+    </row>
+    <row r="148" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A148" s="64" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="5" t="s">
+      <c r="B148" s="17" t="s">
         <v>514</v>
       </c>
-      <c r="B147" s="59"/>
-      <c r="C147" s="5" t="s">
+      <c r="C148" s="8" t="s">
         <v>515</v>
       </c>
-      <c r="D147" s="7" t="s">
+      <c r="D148" s="10" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="75" t="s">
+    <row r="149" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A149" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="B148" s="18" t="s">
+      <c r="B149" s="65" t="s">
         <v>518</v>
       </c>
-      <c r="C148" s="8" t="s">
+      <c r="C149" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="D148" s="10" t="s">
+      <c r="D149" s="2" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="76" t="s">
+    <row r="150" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A150" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="B149" s="77" t="s">
+      <c r="B150" s="65" t="s">
         <v>522</v>
       </c>
-      <c r="C149" s="76" t="s">
+      <c r="C150" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D150" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="D149" s="78" t="s">
+    </row>
+    <row r="151" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A151" s="2" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="78" t="s">
+      <c r="B151" s="66" t="s">
         <v>525</v>
       </c>
-      <c r="B150" s="77" t="s">
+      <c r="C151" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="C150" s="78" t="s">
-        <v>525</v>
-      </c>
-      <c r="D150" s="78" t="s">
+      <c r="D151" s="2" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="78" t="s">
-        <v>528</v>
-      </c>
-      <c r="B151" s="79" t="s">
-        <v>529</v>
-      </c>
-      <c r="C151" s="78" t="s">
-        <v>530</v>
-      </c>
-      <c r="D151" s="78" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="152" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="153" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="154" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="155" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="156" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="157" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="158" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="159" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="160" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="161" ht="15.75" customHeight="1"/>
     <row r="162" ht="15.75" customHeight="1"/>
     <row r="163" ht="15.75" customHeight="1"/>
@@ -5678,129 +5776,128 @@
     <row r="1081" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="D5"/>
-    <hyperlink r:id="rId6" ref="B6"/>
-    <hyperlink r:id="rId7" ref="D6"/>
-    <hyperlink r:id="rId8" ref="B7"/>
-    <hyperlink r:id="rId9" ref="B8"/>
-    <hyperlink r:id="rId10" ref="B9"/>
-    <hyperlink r:id="rId11" ref="B11"/>
-    <hyperlink r:id="rId12" ref="B12"/>
-    <hyperlink r:id="rId13" ref="B13"/>
-    <hyperlink r:id="rId14" ref="D13"/>
-    <hyperlink r:id="rId15" ref="B14"/>
-    <hyperlink r:id="rId16" ref="B15"/>
-    <hyperlink r:id="rId17" ref="B16"/>
-    <hyperlink r:id="rId18" ref="B17"/>
-    <hyperlink r:id="rId19" ref="D17"/>
-    <hyperlink r:id="rId20" ref="B18"/>
-    <hyperlink r:id="rId21" ref="D18"/>
-    <hyperlink r:id="rId22" ref="B19"/>
-    <hyperlink r:id="rId23" ref="B20"/>
-    <hyperlink r:id="rId24" ref="B21"/>
-    <hyperlink r:id="rId25" ref="B22"/>
-    <hyperlink r:id="rId26" ref="B25"/>
-    <hyperlink r:id="rId27" ref="B26"/>
-    <hyperlink r:id="rId28" ref="D26"/>
-    <hyperlink r:id="rId29" ref="B27"/>
-    <hyperlink r:id="rId30" ref="B28"/>
-    <hyperlink r:id="rId31" ref="D28"/>
-    <hyperlink r:id="rId32" ref="B29"/>
-    <hyperlink r:id="rId33" ref="B30"/>
-    <hyperlink r:id="rId34" ref="B31"/>
-    <hyperlink r:id="rId35" ref="B32"/>
-    <hyperlink r:id="rId36" ref="B33"/>
-    <hyperlink r:id="rId37" ref="B34"/>
-    <hyperlink r:id="rId38" ref="B35"/>
-    <hyperlink r:id="rId39" ref="B36"/>
-    <hyperlink r:id="rId40" ref="B37"/>
-    <hyperlink r:id="rId41" ref="B38"/>
-    <hyperlink r:id="rId42" ref="B39"/>
-    <hyperlink r:id="rId43" ref="B40"/>
-    <hyperlink r:id="rId44" ref="B41"/>
-    <hyperlink r:id="rId45" ref="B42"/>
-    <hyperlink r:id="rId46" ref="B43"/>
-    <hyperlink r:id="rId47" ref="D43"/>
-    <hyperlink r:id="rId48" ref="B44"/>
-    <hyperlink r:id="rId49" ref="B46"/>
-    <hyperlink r:id="rId50" ref="B47"/>
-    <hyperlink r:id="rId51" ref="B48"/>
-    <hyperlink r:id="rId52" ref="D48"/>
-    <hyperlink r:id="rId53" ref="B49"/>
-    <hyperlink r:id="rId54" ref="B50"/>
-    <hyperlink r:id="rId55" ref="D50"/>
-    <hyperlink r:id="rId56" ref="B51"/>
-    <hyperlink r:id="rId57" ref="D51"/>
-    <hyperlink r:id="rId58" ref="B52"/>
-    <hyperlink r:id="rId59" ref="B54"/>
-    <hyperlink r:id="rId60" ref="D54"/>
-    <hyperlink r:id="rId61" ref="B56"/>
-    <hyperlink r:id="rId62" ref="B57"/>
-    <hyperlink r:id="rId63" ref="B61"/>
-    <hyperlink r:id="rId64" ref="D61"/>
-    <hyperlink r:id="rId65" ref="B62"/>
-    <hyperlink r:id="rId66" ref="B64"/>
-    <hyperlink r:id="rId67" ref="B65"/>
-    <hyperlink r:id="rId68" ref="B71"/>
-    <hyperlink r:id="rId69" ref="B72"/>
-    <hyperlink r:id="rId70" ref="B73"/>
-    <hyperlink r:id="rId71" ref="B75"/>
-    <hyperlink r:id="rId72" ref="B77"/>
-    <hyperlink r:id="rId73" ref="B80"/>
-    <hyperlink r:id="rId74" ref="B82"/>
-    <hyperlink r:id="rId75" ref="B83"/>
-    <hyperlink r:id="rId76" ref="B85"/>
-    <hyperlink r:id="rId77" ref="B86"/>
-    <hyperlink r:id="rId78" ref="B87"/>
-    <hyperlink r:id="rId79" ref="D87"/>
-    <hyperlink r:id="rId80" ref="B88"/>
-    <hyperlink r:id="rId81" ref="B91"/>
-    <hyperlink r:id="rId82" ref="B92"/>
-    <hyperlink r:id="rId83" ref="D92"/>
-    <hyperlink r:id="rId84" ref="B94"/>
-    <hyperlink r:id="rId85" ref="B95"/>
-    <hyperlink r:id="rId86" ref="B96"/>
-    <hyperlink r:id="rId87" ref="B105"/>
-    <hyperlink r:id="rId88" ref="B107"/>
-    <hyperlink r:id="rId89" ref="B110"/>
-    <hyperlink r:id="rId90" ref="B112"/>
-    <hyperlink r:id="rId91" ref="B114"/>
-    <hyperlink r:id="rId92" ref="B115"/>
-    <hyperlink r:id="rId93" ref="B117"/>
-    <hyperlink r:id="rId94" ref="B118"/>
-    <hyperlink r:id="rId95" ref="B120"/>
-    <hyperlink r:id="rId96" ref="D120"/>
-    <hyperlink r:id="rId97" ref="B122"/>
-    <hyperlink r:id="rId98" ref="B127"/>
-    <hyperlink r:id="rId99" ref="B128"/>
-    <hyperlink r:id="rId100" ref="B130"/>
-    <hyperlink r:id="rId101" ref="D130"/>
-    <hyperlink r:id="rId102" ref="B131"/>
-    <hyperlink r:id="rId103" ref="B132"/>
-    <hyperlink r:id="rId104" ref="B133"/>
-    <hyperlink r:id="rId105" ref="B134"/>
-    <hyperlink r:id="rId106" ref="B138"/>
-    <hyperlink r:id="rId107" ref="B139"/>
-    <hyperlink r:id="rId108" ref="B140"/>
-    <hyperlink r:id="rId109" ref="B141"/>
-    <hyperlink r:id="rId110" ref="B143"/>
-    <hyperlink r:id="rId111" ref="B146"/>
-    <hyperlink r:id="rId112" ref="B148"/>
-    <hyperlink r:id="rId113" ref="D148"/>
-    <hyperlink r:id="rId114" ref="B149"/>
-    <hyperlink r:id="rId115" ref="B150"/>
-    <hyperlink r:id="rId116" ref="B151"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D13" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B14" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B15" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B16" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B17" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D17" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B18" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D18" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B19" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B20" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B21" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B22" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B25" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B26" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D26" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B27" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B28" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="D28" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B29" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B30" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B31" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B33" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B34" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B35" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B36" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B37" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B38" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B39" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B40" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B41" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B42" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B43" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D43" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B44" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B46" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B47" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B48" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="D48" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B49" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B50" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="D50" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B51" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="D51" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B52" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B54" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="D54" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B56" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B57" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B61" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="D61" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B62" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B64" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B65" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B71" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B72" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B73" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B75" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B80" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B82" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B83" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B85" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B86" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B87" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="D87" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B88" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B91" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B92" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="D92" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B94" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B95" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B96" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B105" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B107" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B110" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B112" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B114" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B115" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B117" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B118" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B120" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="D120" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B122" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B127" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B128" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B130" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="D130" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B131" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B132" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B133" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B134" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="B138" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="B139" r:id="rId105" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="B140" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="B141" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="B143" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="B146" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="B148" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="D148" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="B149" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="B150" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="B151" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="B55" r:id="rId115" display="https://reconcile.gnd.network/gnd/4142078-0" xr:uid="{B8894048-7ABE-4D4D-8C7A-CA8FEB064ED8}"/>
+    <hyperlink ref="B76" r:id="rId116" display="https://reconcile.gnd.network/gnd/4777777-1" xr:uid="{0339D8C4-8531-904F-B5E1-CE32AEDE7C8A}"/>
+    <hyperlink ref="B137" r:id="rId117" display="https://reconcile.gnd.network/gnd/4271516-7" xr:uid="{131A5B64-43BD-934F-A89A-71B867E96CB7}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.787401575"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId117"/>
   <tableParts count="1">
-    <tablePart r:id="rId119"/>
+    <tablePart r:id="rId118"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>